<commit_message>
Updated test data sheet for 40V test case
</commit_message>
<xml_diff>
--- a/Test Data/Verify_40V_Calculation_For_PFI_with_Devices.xlsx
+++ b/Test Data/Verify_40V_Calculation_For_PFI_with_Devices.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbhosash\Desktop\31st Jan\NGConsys Automation\Test Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A2AAE50-1EFB-4C08-9763-8D8978CC792E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13800" windowHeight="5604"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Add Panels" sheetId="6" r:id="rId1"/>
@@ -159,9 +160,6 @@
     <t>0.055</t>
   </si>
   <si>
-    <t>Pro215s</t>
-  </si>
-  <si>
     <t>Loop Index</t>
   </si>
   <si>
@@ -181,12 +179,15 @@
   </si>
   <si>
     <t>FV 411 F</t>
+  </si>
+  <si>
+    <t>Pro215S</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -639,11 +640,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -740,10 +741,10 @@
       <c r="L6" s="22"/>
       <c r="M6" s="23"/>
       <c r="O6" s="16" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="P6" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
@@ -769,7 +770,7 @@
         <v>40</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I7" s="14"/>
       <c r="J7" s="11" t="s">
@@ -830,10 +831,10 @@
         <v>25</v>
       </c>
       <c r="O8" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.3">
@@ -863,15 +864,15 @@
       </c>
       <c r="I9" s="14"/>
       <c r="O9" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="P9" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>10</v>
@@ -907,7 +908,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
@@ -998,7 +999,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -1095,5 +1096,6 @@
     <mergeCell ref="C2:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>